<commit_message>
Incorporación de observaciones FRLP
</commit_message>
<xml_diff>
--- a/2022/Formulario-Memoria_VF-2022.xlsx
+++ b/2022/Formulario-Memoria_VF-2022.xlsx
@@ -758,6 +758,11 @@
   </si>
   <si>
     <t xml:space="preserve">Las actividades planificadas para el año 2023 son: 
+ Continuar con el desarrollo de los proyectos en ejecución:
+ - PID MAUTILP0007746TC: Caracterizar las cadenas de fuerzas en granos con forma pentagonal en el fenómeno de stick-slip  en una geometría Couette, y comparar con los resultados obtenidos para discos. Estudiar la formación de agregados magnéticos en sistemas confinados en dos dimensiones, mediante simulaciones computacionales y experimentos.
+ - PICT-2020-SERIEA-I-GRF-00457: Se realizarán mediciones de calibración con el prototipo desarrollado en medios canónicos (respuesta dieléctrica conocida) y se contrastarán con resultados analíticos y de simulación. Asimismo, se continuará con el desarrollo del software  de métodos directo e inverso.
+ - PICT-2020-SERIEA-I-GRF-02611: Se avanzará en la caracterización del estado tensional de silos con paredes lisas y rugosas, tanto experimentalmente como a través de simulaciones computacionales.
+ - PIP 11220200100717CO: Se desarrollarán experimentos para el análisis del estado tensional y estructural de descarga forzada de silos con diferentes configuraciones de llenado. Se intentará modelar computacionalmente estas configuraciones para obtener resultados numéricos complementarios. 
  Redactar y publicar al menos seis trabajos en revistas internacionales con referato, producto de las investigaciones en las líneas de trabajo actualmente en desarrollo en el GMG. 
  Participar en al menos tres congresos nacionales y uno internacional. 
  Progresar en el desarrollo de los planes de tesis doctorales en curso. 
@@ -1035,7 +1040,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1146,8 +1151,8 @@
   </sheetPr>
   <dimension ref="A1:J410"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A368" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A389" activeCellId="0" sqref="A389"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A373" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J388" activeCellId="0" sqref="J388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1766,7 +1771,7 @@
         <v>23</v>
       </c>
       <c r="F41" s="11" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -6451,11 +6456,6 @@
       <c r="A365" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B365" s="0"/>
-      <c r="C365" s="0"/>
-      <c r="D365" s="0"/>
-      <c r="E365" s="0"/>
-      <c r="F365" s="0"/>
       <c r="G365" s="3"/>
       <c r="H365" s="3"/>
       <c r="I365" s="3"/>
@@ -6773,7 +6773,7 @@
       <c r="I382" s="3"/>
       <c r="J382" s="3"/>
     </row>
-    <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="383" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A383" s="8" t="s">
         <v>245</v>
       </c>
@@ -6787,7 +6787,7 @@
       <c r="I383" s="3"/>
       <c r="J383" s="3"/>
     </row>
-    <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="384" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A384" s="8"/>
       <c r="B384" s="8"/>
       <c r="C384" s="8"/>
@@ -6811,7 +6811,7 @@
       <c r="I385" s="3"/>
       <c r="J385" s="3"/>
     </row>
-    <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="386" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A386" s="8"/>
       <c r="B386" s="8"/>
       <c r="C386" s="8"/>
@@ -6835,7 +6835,7 @@
       <c r="I387" s="3"/>
       <c r="J387" s="3"/>
     </row>
-    <row r="388" customFormat="false" ht="126.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="388" customFormat="false" ht="174.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A388" s="8"/>
       <c r="B388" s="8"/>
       <c r="C388" s="8"/>

</xml_diff>